<commit_message>
registro de pagamento e planejamento base das rotinas
</commit_message>
<xml_diff>
--- a/storage/Planilha_Controle_Despesas_v2601_1.xlsx
+++ b/storage/Planilha_Controle_Despesas_v2601_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\obsidian\heleri\storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\heleri\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8BAD6D-4582-46C5-B3E3-5F278CCF42D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAC0657-EB15-4C56-AB9F-21816D78848F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{18AB48FE-6D0A-408B-81DD-88C3E4CE2477}"/>
+    <workbookView xWindow="-28920" yWindow="-2910" windowWidth="29040" windowHeight="15840" xr2:uid="{18AB48FE-6D0A-408B-81DD-88C3E4CE2477}"/>
   </bookViews>
   <sheets>
     <sheet name="2601" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -104,13 +104,23 @@
   </si>
   <si>
     <t>Q260121_2116 Ausência Mangueira Incêndio Hall Andar 4</t>
+  </si>
+  <si>
+    <t>Valdeci</t>
+  </si>
+  <si>
+    <t>cobrir férias Rogerio</t>
+  </si>
+  <si>
+    <t>260203_Comprovante_Pgto_Valdeci_Servicos_Jan_2026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;R$&quot;\ #,##0;[Red]\-&quot;R$&quot;\ #,##0"/>
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
@@ -194,7 +204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,6 +234,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -541,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE75F61D-5328-424E-AC09-9079298705BC}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +569,7 @@
     <col min="4" max="4" width="15.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" style="4" customWidth="1"/>
     <col min="8" max="8" width="23.5703125" style="4" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="5" customWidth="1"/>
   </cols>
@@ -568,15 +581,15 @@
       </c>
       <c r="E1" s="8">
         <f>SUM(E3:E600)</f>
-        <v>670.64</v>
+        <v>1020.64</v>
       </c>
       <c r="F1" s="5">
         <f>COUNTA(F3:F600)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="5">
         <f>COUNTA(G3:G600)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" s="5">
         <f>COUNTA(H3:H600)</f>
@@ -584,7 +597,7 @@
       </c>
       <c r="I1" s="5">
         <f>COUNTIF(I3:I600,"sim")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -729,6 +742,29 @@
         <v>23</v>
       </c>
       <c r="I6" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="11">
+        <v>46056</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="13">
+        <v>350</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>